<commit_message>
include $ as an equivalent of piasses
</commit_message>
<xml_diff>
--- a/results/wer_corpusgen.xlsx
+++ b/results/wer_corpusgen.xlsx
@@ -502,23 +502,23 @@
         </is>
       </c>
       <c r="D2" t="n">
+        <v>0.08571428571428572</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>non je l'attends par la poste moi je vais payer dix pièces euh je voudrais savoir si c'est confirmé si ça a été payé je l'ai fait par accéder là</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>0.1714285714285714</v>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Non, je l'attends par la poste. Moi, je viens de payer 10 pièces. Je voudrais savoir si c'est confirmé, si ça a été payé, je l'ai fait par accéder là .</t>
+        </is>
+      </c>
+      <c r="H2" t="n">
         <v>0.1142857142857143</v>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>non je l'attends par la poste moi je vais payer dix pièces euh je voudrais savoir si c'est confirmé si ça a été payé je l'ai fait par accéder là</t>
-        </is>
-      </c>
-      <c r="F2" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>Non, je l'attends par la poste. Moi, je viens de payer 10 pièces. Je voudrais savoir si c'est confirmé, si ça a été payé, je l'ai fait par accéder là .</t>
-        </is>
-      </c>
-      <c r="H2" t="n">
-        <v>0.1428571428571428</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
@@ -546,7 +546,7 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>0.2</v>
+        <v>0.1714285714285714</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -554,7 +554,7 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>0.2571428571428571</v>
+        <v>0.2285714285714286</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
@@ -590,7 +590,7 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>0.1714285714285714</v>
+        <v>0.1428571428571428</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -598,7 +598,7 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>0.3428571428571429</v>
+        <v>0.3142857142857143</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
@@ -7302,7 +7302,7 @@
         </is>
       </c>
       <c r="J156" t="n">
-        <v>0.1428571428571428</v>
+        <v>0.07142857142857142</v>
       </c>
     </row>
     <row r="157">
@@ -7346,7 +7346,7 @@
         </is>
       </c>
       <c r="J157" t="n">
-        <v>0.1428571428571428</v>
+        <v>0.07142857142857142</v>
       </c>
     </row>
     <row r="158">
@@ -11942,7 +11942,7 @@
         </is>
       </c>
       <c r="D262" t="n">
-        <v>0.1296296296296296</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="E262" t="inlineStr">
         <is>
@@ -17318,7 +17318,7 @@
         </is>
       </c>
       <c r="F384" t="n">
-        <v>0.1680672268907563</v>
+        <v>0.1596638655462185</v>
       </c>
       <c r="G384" t="inlineStr">
         <is>
@@ -17326,7 +17326,7 @@
         </is>
       </c>
       <c r="H384" t="n">
-        <v>0.1512605042016807</v>
+        <v>0.1428571428571428</v>
       </c>
       <c r="I384" t="inlineStr">
         <is>
@@ -17362,7 +17362,7 @@
         </is>
       </c>
       <c r="F385" t="n">
-        <v>0.2016806722689076</v>
+        <v>0.1932773109243698</v>
       </c>
       <c r="G385" t="inlineStr">
         <is>
@@ -17406,7 +17406,7 @@
         </is>
       </c>
       <c r="F386" t="n">
-        <v>0.1680672268907563</v>
+        <v>0.1596638655462185</v>
       </c>
       <c r="G386" t="inlineStr">
         <is>

</xml_diff>